<commit_message>
4.0.1.7 and 4.0.1.8 updates
</commit_message>
<xml_diff>
--- a/WaterskiScoringSystem/WaterskiScoringSystem/RecordApplicationFormTemplate.xlsx
+++ b/WaterskiScoringSystem/WaterskiScoringSystem/RecordApplicationFormTemplate.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WaterskiScoring\VisualStudioProjects\WaterskiScoringSystem\WaterskiScoringSystem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WaterskiScoring\GitHub\WaterskiScoringSystem\WaterskiScoringSystem\WaterskiScoringSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -138,9 +138,6 @@
     <t>Year:</t>
   </si>
   <si>
-    <t>Manfacture:</t>
-  </si>
-  <si>
     <t>Make &amp; Model:</t>
   </si>
   <si>
@@ -364,6 +361,9 @@
   </si>
   <si>
     <t xml:space="preserve">To the best of our knowledge, all current AWSA rules and record specifications ( except as noted ) were followed, </t>
+  </si>
+  <si>
+    <t>Manufacture:</t>
   </si>
 </sst>
 </file>
@@ -653,86 +653,107 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -744,12 +765,7 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -778,22 +794,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -829,7 +829,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1042" name="Picture 8" descr="AWSA"/>
+        <xdr:cNvPr id="1042" name="Picture 8" descr="AWSA">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1274,24 +1280,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="26.25">
-      <c r="A1" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
+      <c r="A1" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1">
-      <c r="A2" s="39"/>
+      <c r="A2" s="47"/>
       <c r="B2" s="40"/>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
@@ -1306,21 +1312,21 @@
       <c r="M2" s="40"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="18">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="40"/>
@@ -1338,21 +1344,21 @@
       <c r="M4" s="40"/>
     </row>
     <row r="5" spans="1:13" ht="18">
-      <c r="A5" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
+      <c r="A5" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="40"/>
@@ -1370,106 +1376,106 @@
       <c r="M6" s="40"/>
     </row>
     <row r="7" spans="1:13" ht="15">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+    </row>
+    <row r="8" spans="1:13" ht="48" customHeight="1">
+      <c r="A8" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="37"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+    </row>
+    <row r="10" spans="1:13" ht="15">
+      <c r="A10" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-    </row>
-    <row r="8" spans="1:13" ht="48" customHeight="1">
-      <c r="A8" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-    </row>
-    <row r="10" spans="1:13" ht="15">
-      <c r="A10" s="37" t="s">
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+    </row>
+    <row r="11" spans="1:13" ht="36" customHeight="1">
+      <c r="A11" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="37"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+    </row>
+    <row r="13" spans="1:13" ht="15">
+      <c r="A13" s="39" t="s">
         <v>44</v>
-      </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-    </row>
-    <row r="11" spans="1:13" ht="36" customHeight="1">
-      <c r="A11" s="48" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-    </row>
-    <row r="13" spans="1:13" ht="15">
-      <c r="A13" s="37" t="s">
-        <v>45</v>
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="40"/>
@@ -1485,40 +1491,40 @@
       <c r="M13" s="40"/>
     </row>
     <row r="14" spans="1:13" ht="24" customHeight="1">
-      <c r="A14" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
+      <c r="A14" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="36"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
     </row>
     <row r="16" spans="1:13" ht="15">
-      <c r="A16" s="35" t="s">
-        <v>57</v>
+      <c r="A16" s="41" t="s">
+        <v>56</v>
       </c>
       <c r="B16" s="40"/>
       <c r="C16" s="40"/>
@@ -1534,40 +1540,40 @@
       <c r="M16" s="40"/>
     </row>
     <row r="17" spans="1:13" ht="24" customHeight="1">
-      <c r="A17" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
+      <c r="A17" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
     </row>
     <row r="18" spans="1:13" ht="15">
-      <c r="A18" s="35"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
     </row>
     <row r="19" spans="1:13" ht="15">
-      <c r="A19" s="37" t="s">
-        <v>46</v>
+      <c r="A19" s="39" t="s">
+        <v>45</v>
       </c>
       <c r="B19" s="40"/>
       <c r="C19" s="40"/>
@@ -1583,284 +1589,304 @@
       <c r="M19" s="40"/>
     </row>
     <row r="20" spans="1:13" ht="48" customHeight="1">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+    </row>
+    <row r="22" spans="1:13" ht="15">
+      <c r="A22" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+    </row>
+    <row r="23" spans="1:13" ht="48" customHeight="1">
+      <c r="A23" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="37"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+    </row>
+    <row r="25" spans="1:13" ht="15">
+      <c r="A25" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+    </row>
+    <row r="26" spans="1:13" ht="60" customHeight="1">
+      <c r="A26" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="37"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
+    </row>
+    <row r="28" spans="1:13" ht="15">
+      <c r="A28" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="37"/>
+      <c r="M28" s="37"/>
+    </row>
+    <row r="29" spans="1:13" ht="36" customHeight="1">
+      <c r="A29" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="37"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="37"/>
+      <c r="M30" s="37"/>
+    </row>
+    <row r="31" spans="1:13" ht="60" customHeight="1">
+      <c r="A31" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="44"/>
+      <c r="L31" s="44"/>
+      <c r="M31" s="44"/>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="37"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+    </row>
+    <row r="33" spans="1:13" ht="15">
+      <c r="A33" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="37"/>
+      <c r="M33" s="37"/>
+    </row>
+    <row r="34" spans="1:13" ht="108" customHeight="1">
+      <c r="A34" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="48"/>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="36"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-    </row>
-    <row r="22" spans="1:13" ht="15">
-      <c r="A22" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
-    </row>
-    <row r="23" spans="1:13" ht="48" customHeight="1">
-      <c r="A23" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="47"/>
-      <c r="M23" s="47"/>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="36"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-    </row>
-    <row r="25" spans="1:13" ht="15">
-      <c r="A25" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="36"/>
-    </row>
-    <row r="26" spans="1:13" ht="60" customHeight="1">
-      <c r="A26" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="47"/>
-      <c r="K26" s="47"/>
-      <c r="L26" s="47"/>
-      <c r="M26" s="47"/>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="36"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="36"/>
-    </row>
-    <row r="28" spans="1:13" ht="15">
-      <c r="A28" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="36"/>
-      <c r="M28" s="36"/>
-    </row>
-    <row r="29" spans="1:13" ht="36" customHeight="1">
-      <c r="A29" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47"/>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="36"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="36"/>
-      <c r="K30" s="36"/>
-      <c r="L30" s="36"/>
-      <c r="M30" s="36"/>
-    </row>
-    <row r="31" spans="1:13" ht="60" customHeight="1">
-      <c r="A31" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
-      <c r="M31" s="43"/>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="36"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="36"/>
-    </row>
-    <row r="33" spans="1:13" ht="15">
-      <c r="A33" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="36"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="36"/>
-      <c r="M33" s="36"/>
-    </row>
-    <row r="34" spans="1:13" ht="108" customHeight="1">
-      <c r="A34" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="48"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="48"/>
-      <c r="M34" s="48"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="38"/>
+      <c r="L34" s="38"/>
+      <c r="M34" s="38"/>
     </row>
     <row r="35" spans="1:13">
-      <c r="A35" s="36"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="36"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="44"/>
-      <c r="K36" s="44"/>
-      <c r="L36" s="44"/>
-      <c r="M36" s="44"/>
+      <c r="A36" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="45"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="45"/>
+      <c r="M36" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A18:M18"/>
+    <mergeCell ref="A21:M21"/>
+    <mergeCell ref="A24:M24"/>
+    <mergeCell ref="A7:M7"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="A9:M9"/>
+    <mergeCell ref="A12:M12"/>
+    <mergeCell ref="A15:M15"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A6:M6"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A30:M30"/>
+    <mergeCell ref="A31:M31"/>
+    <mergeCell ref="A35:M35"/>
+    <mergeCell ref="A36:M36"/>
+    <mergeCell ref="A28:M28"/>
+    <mergeCell ref="A33:M33"/>
     <mergeCell ref="A26:M26"/>
     <mergeCell ref="A29:M29"/>
     <mergeCell ref="A32:M32"/>
@@ -1877,26 +1903,6 @@
     <mergeCell ref="A20:M20"/>
     <mergeCell ref="A23:M23"/>
     <mergeCell ref="A27:M27"/>
-    <mergeCell ref="A30:M30"/>
-    <mergeCell ref="A31:M31"/>
-    <mergeCell ref="A35:M35"/>
-    <mergeCell ref="A36:M36"/>
-    <mergeCell ref="A28:M28"/>
-    <mergeCell ref="A33:M33"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A6:M6"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A18:M18"/>
-    <mergeCell ref="A21:M21"/>
-    <mergeCell ref="A24:M24"/>
-    <mergeCell ref="A7:M7"/>
-    <mergeCell ref="A10:M10"/>
-    <mergeCell ref="A9:M9"/>
-    <mergeCell ref="A12:M12"/>
-    <mergeCell ref="A15:M15"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1912,8 +1918,8 @@
   </sheetPr>
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18:H18"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12"/>
@@ -1935,19 +1941,19 @@
     </row>
     <row r="2" spans="1:8" ht="26.25">
       <c r="B2" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:8" ht="18" customHeight="1"/>
     <row r="4" spans="1:8" ht="18" customHeight="1">
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1990,7 +1996,7 @@
     </row>
     <row r="9" spans="1:8" ht="15">
       <c r="A9" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
@@ -2048,8 +2054,8 @@
       <c r="F14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="49"/>
-      <c r="H14" s="51"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="55"/>
     </row>
     <row r="15" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A15" s="5"/>
@@ -2063,8 +2069,8 @@
       <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="74"/>
-      <c r="D16" s="75"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="65"/>
       <c r="F16" s="6" t="s">
         <v>11</v>
       </c>
@@ -2084,14 +2090,14 @@
         <v>12</v>
       </c>
       <c r="B18" s="5"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="51"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="55"/>
       <c r="F18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="76"/>
-      <c r="H18" s="77"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="57"/>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A19" s="5"/>
@@ -2104,10 +2110,10 @@
       <c r="A20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="51"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="55"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
@@ -2135,14 +2141,14 @@
       <c r="A23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="49"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="51"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="55"/>
       <c r="E23" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="49"/>
-      <c r="G23" s="51"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="55"/>
     </row>
     <row r="24" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A24" s="5"/>
@@ -2155,7 +2161,7 @@
     </row>
     <row r="25" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A25" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="58"/>
       <c r="C25" s="59"/>
@@ -2183,8 +2189,8 @@
       <c r="E27" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="61"/>
-      <c r="G27" s="62"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="67"/>
     </row>
     <row r="28" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A28" s="5"/>
@@ -2199,11 +2205,11 @@
       <c r="A29" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="49"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="51"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="55"/>
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:8" ht="18" customHeight="1" thickBot="1">
@@ -2217,7 +2223,7 @@
     </row>
     <row r="31" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A31" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B31" s="27"/>
       <c r="C31" s="27"/>
@@ -2243,32 +2249,32 @@
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
       <c r="E33" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A34" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" s="53"/>
-      <c r="C34" s="54"/>
+        <v>36</v>
+      </c>
+      <c r="B34" s="61"/>
+      <c r="C34" s="62"/>
       <c r="D34" s="13"/>
       <c r="E34" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F34" s="49"/>
-      <c r="G34" s="51"/>
+        <v>100</v>
+      </c>
+      <c r="F34" s="54"/>
+      <c r="G34" s="55"/>
     </row>
     <row r="35" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A35" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="53"/>
-      <c r="C35" s="54"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="62"/>
       <c r="D35" s="13"/>
       <c r="E35" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="16"/>
@@ -2293,8 +2299,8 @@
       <c r="G37" s="5"/>
     </row>
     <row r="38" spans="1:8" ht="18" customHeight="1">
-      <c r="A38" s="55" t="s">
-        <v>100</v>
+      <c r="A38" s="68" t="s">
+        <v>99</v>
       </c>
       <c r="B38" s="40"/>
       <c r="C38" s="40"/>
@@ -2304,8 +2310,8 @@
       <c r="G38" s="40"/>
     </row>
     <row r="39" spans="1:8" ht="18" customHeight="1">
-      <c r="A39" s="55" t="s">
-        <v>50</v>
+      <c r="A39" s="68" t="s">
+        <v>49</v>
       </c>
       <c r="B39" s="40"/>
       <c r="C39" s="40"/>
@@ -2315,8 +2321,8 @@
       <c r="G39" s="40"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1">
-      <c r="A40" s="55" t="s">
-        <v>52</v>
+      <c r="A40" s="68" t="s">
+        <v>51</v>
       </c>
       <c r="B40" s="40"/>
       <c r="C40" s="40"/>
@@ -2365,11 +2371,11 @@
       <c r="A44" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B44" s="52"/>
-      <c r="C44" s="52"/>
-      <c r="D44" s="52"/>
-      <c r="E44" s="52"/>
-      <c r="F44" s="52"/>
+      <c r="B44" s="51"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
       <c r="G44" s="20"/>
       <c r="H44" s="23"/>
     </row>
@@ -2387,18 +2393,18 @@
       <c r="A46" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="52"/>
-      <c r="C46" s="52"/>
-      <c r="D46" s="52"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="57"/>
+      <c r="B46" s="51"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="53"/>
       <c r="G46" s="19"/>
       <c r="H46" s="23"/>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A47" s="5"/>
       <c r="B47" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -2411,11 +2417,11 @@
       <c r="A48" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B48" s="52"/>
-      <c r="C48" s="52"/>
-      <c r="D48" s="52"/>
-      <c r="E48" s="52"/>
-      <c r="F48" s="52"/>
+      <c r="B48" s="51"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="51"/>
       <c r="G48" s="23"/>
       <c r="H48" s="23"/>
     </row>
@@ -2433,11 +2439,11 @@
       <c r="A50" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B50" s="52"/>
-      <c r="C50" s="52"/>
-      <c r="D50" s="52"/>
-      <c r="E50" s="52"/>
-      <c r="F50" s="52"/>
+      <c r="B50" s="51"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="51"/>
       <c r="G50" s="23"/>
       <c r="H50" s="23"/>
     </row>
@@ -2466,7 +2472,7 @@
     <row r="53" spans="1:8" ht="18" customHeight="1">
       <c r="A53" s="3"/>
       <c r="B53" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="6" t="s">
@@ -2475,350 +2481,310 @@
     </row>
     <row r="54" spans="1:8" ht="18" customHeight="1">
       <c r="A54" s="24"/>
-      <c r="B54" s="63"/>
-      <c r="C54" s="64"/>
+      <c r="B54" s="49"/>
+      <c r="C54" s="50"/>
       <c r="D54" s="25"/>
     </row>
     <row r="55" spans="1:8" ht="18" customHeight="1">
       <c r="A55" s="24"/>
-      <c r="B55" s="63"/>
-      <c r="C55" s="64"/>
+      <c r="B55" s="49"/>
+      <c r="C55" s="50"/>
       <c r="D55" s="25"/>
     </row>
     <row r="56" spans="1:8" ht="18" customHeight="1">
       <c r="A56" s="24"/>
-      <c r="B56" s="63"/>
-      <c r="C56" s="64"/>
+      <c r="B56" s="49"/>
+      <c r="C56" s="50"/>
       <c r="D56" s="25"/>
     </row>
     <row r="57" spans="1:8" ht="18" customHeight="1">
       <c r="A57" s="24"/>
-      <c r="B57" s="63"/>
-      <c r="C57" s="64"/>
+      <c r="B57" s="49"/>
+      <c r="C57" s="50"/>
       <c r="D57" s="25"/>
     </row>
     <row r="58" spans="1:8" ht="18" customHeight="1">
       <c r="A58" s="24"/>
-      <c r="B58" s="63"/>
-      <c r="C58" s="64"/>
+      <c r="B58" s="49"/>
+      <c r="C58" s="50"/>
       <c r="D58" s="25"/>
     </row>
     <row r="59" spans="1:8" ht="18" customHeight="1">
       <c r="A59" s="24"/>
-      <c r="B59" s="63"/>
-      <c r="C59" s="64"/>
+      <c r="B59" s="49"/>
+      <c r="C59" s="50"/>
       <c r="D59" s="25"/>
     </row>
     <row r="60" spans="1:8" ht="18" customHeight="1">
       <c r="A60" s="24"/>
-      <c r="B60" s="63"/>
-      <c r="C60" s="64"/>
+      <c r="B60" s="49"/>
+      <c r="C60" s="50"/>
       <c r="D60" s="25"/>
     </row>
     <row r="61" spans="1:8" ht="18" customHeight="1">
       <c r="A61" s="24"/>
-      <c r="B61" s="63"/>
-      <c r="C61" s="64"/>
+      <c r="B61" s="49"/>
+      <c r="C61" s="50"/>
       <c r="D61" s="25"/>
     </row>
     <row r="62" spans="1:8" ht="18" customHeight="1">
       <c r="A62" s="24"/>
-      <c r="B62" s="63"/>
-      <c r="C62" s="64"/>
+      <c r="B62" s="49"/>
+      <c r="C62" s="50"/>
       <c r="D62" s="25"/>
     </row>
     <row r="63" spans="1:8" ht="18" customHeight="1">
       <c r="A63" s="24"/>
-      <c r="B63" s="63"/>
-      <c r="C63" s="64"/>
+      <c r="B63" s="49"/>
+      <c r="C63" s="50"/>
       <c r="D63" s="25"/>
     </row>
     <row r="64" spans="1:8" ht="18" customHeight="1">
       <c r="A64" s="24"/>
-      <c r="B64" s="63"/>
-      <c r="C64" s="64"/>
+      <c r="B64" s="49"/>
+      <c r="C64" s="50"/>
       <c r="D64" s="25"/>
     </row>
     <row r="65" spans="1:4" ht="18" customHeight="1">
       <c r="A65" s="24"/>
-      <c r="B65" s="63"/>
-      <c r="C65" s="64"/>
+      <c r="B65" s="49"/>
+      <c r="C65" s="50"/>
       <c r="D65" s="25"/>
     </row>
     <row r="66" spans="1:4" ht="18" customHeight="1">
       <c r="A66" s="24"/>
-      <c r="B66" s="63"/>
-      <c r="C66" s="64"/>
+      <c r="B66" s="49"/>
+      <c r="C66" s="50"/>
       <c r="D66" s="25"/>
     </row>
     <row r="67" spans="1:4" ht="18" customHeight="1">
       <c r="A67" s="24"/>
-      <c r="B67" s="63"/>
-      <c r="C67" s="64"/>
+      <c r="B67" s="49"/>
+      <c r="C67" s="50"/>
       <c r="D67" s="25"/>
     </row>
     <row r="68" spans="1:4" ht="18" customHeight="1">
       <c r="A68" s="24"/>
-      <c r="B68" s="63"/>
-      <c r="C68" s="64"/>
+      <c r="B68" s="49"/>
+      <c r="C68" s="50"/>
       <c r="D68" s="25"/>
     </row>
     <row r="69" spans="1:4" ht="18" customHeight="1">
       <c r="A69" s="24"/>
-      <c r="B69" s="63"/>
-      <c r="C69" s="64"/>
+      <c r="B69" s="49"/>
+      <c r="C69" s="50"/>
       <c r="D69" s="25"/>
     </row>
     <row r="70" spans="1:4" ht="18" customHeight="1">
       <c r="A70" s="24"/>
-      <c r="B70" s="63"/>
-      <c r="C70" s="64"/>
+      <c r="B70" s="49"/>
+      <c r="C70" s="50"/>
       <c r="D70" s="25"/>
     </row>
     <row r="71" spans="1:4" ht="18" customHeight="1">
       <c r="A71" s="24"/>
-      <c r="B71" s="63"/>
-      <c r="C71" s="64"/>
+      <c r="B71" s="49"/>
+      <c r="C71" s="50"/>
       <c r="D71" s="25"/>
     </row>
     <row r="72" spans="1:4" ht="18" customHeight="1">
       <c r="A72" s="24"/>
-      <c r="B72" s="63"/>
-      <c r="C72" s="64"/>
+      <c r="B72" s="49"/>
+      <c r="C72" s="50"/>
       <c r="D72" s="25"/>
     </row>
     <row r="73" spans="1:4" ht="18" customHeight="1">
       <c r="A73" s="24"/>
-      <c r="B73" s="63"/>
-      <c r="C73" s="64"/>
+      <c r="B73" s="49"/>
+      <c r="C73" s="50"/>
       <c r="D73" s="25"/>
     </row>
     <row r="74" spans="1:4" ht="18" customHeight="1">
       <c r="A74" s="24"/>
-      <c r="B74" s="63"/>
-      <c r="C74" s="64"/>
+      <c r="B74" s="49"/>
+      <c r="C74" s="50"/>
       <c r="D74" s="25"/>
     </row>
     <row r="75" spans="1:4" ht="18" customHeight="1">
       <c r="A75" s="24"/>
-      <c r="B75" s="63"/>
-      <c r="C75" s="64"/>
+      <c r="B75" s="49"/>
+      <c r="C75" s="50"/>
       <c r="D75" s="25"/>
     </row>
     <row r="76" spans="1:4" ht="18" customHeight="1">
       <c r="A76" s="24"/>
-      <c r="B76" s="63"/>
-      <c r="C76" s="64"/>
+      <c r="B76" s="49"/>
+      <c r="C76" s="50"/>
       <c r="D76" s="25"/>
     </row>
     <row r="77" spans="1:4" ht="18" customHeight="1">
       <c r="A77" s="24"/>
-      <c r="B77" s="63"/>
-      <c r="C77" s="64"/>
+      <c r="B77" s="49"/>
+      <c r="C77" s="50"/>
       <c r="D77" s="25"/>
     </row>
     <row r="78" spans="1:4" ht="18" customHeight="1">
       <c r="A78" s="24"/>
-      <c r="B78" s="63"/>
-      <c r="C78" s="64"/>
+      <c r="B78" s="49"/>
+      <c r="C78" s="50"/>
       <c r="D78" s="25"/>
     </row>
     <row r="79" spans="1:4" ht="18" customHeight="1">
       <c r="A79" s="24"/>
-      <c r="B79" s="63"/>
-      <c r="C79" s="64"/>
+      <c r="B79" s="49"/>
+      <c r="C79" s="50"/>
       <c r="D79" s="25"/>
     </row>
     <row r="80" spans="1:4" ht="18" customHeight="1">
       <c r="A80" s="24"/>
-      <c r="B80" s="63"/>
-      <c r="C80" s="64"/>
+      <c r="B80" s="49"/>
+      <c r="C80" s="50"/>
       <c r="D80" s="25"/>
     </row>
     <row r="81" spans="1:4" ht="18" customHeight="1">
       <c r="A81" s="24"/>
-      <c r="B81" s="63"/>
-      <c r="C81" s="64"/>
+      <c r="B81" s="49"/>
+      <c r="C81" s="50"/>
       <c r="D81" s="25"/>
     </row>
     <row r="82" spans="1:4" ht="18" customHeight="1">
       <c r="A82" s="24"/>
-      <c r="B82" s="63"/>
-      <c r="C82" s="64"/>
+      <c r="B82" s="49"/>
+      <c r="C82" s="50"/>
       <c r="D82" s="25"/>
     </row>
     <row r="83" spans="1:4" ht="18" customHeight="1">
       <c r="A83" s="24"/>
-      <c r="B83" s="63"/>
-      <c r="C83" s="64"/>
+      <c r="B83" s="49"/>
+      <c r="C83" s="50"/>
       <c r="D83" s="25"/>
     </row>
     <row r="84" spans="1:4" ht="18" customHeight="1">
       <c r="A84" s="24"/>
-      <c r="B84" s="63"/>
-      <c r="C84" s="64"/>
+      <c r="B84" s="49"/>
+      <c r="C84" s="50"/>
       <c r="D84" s="25"/>
     </row>
     <row r="85" spans="1:4" ht="18" customHeight="1">
       <c r="A85" s="24"/>
-      <c r="B85" s="63"/>
-      <c r="C85" s="64"/>
+      <c r="B85" s="49"/>
+      <c r="C85" s="50"/>
       <c r="D85" s="25"/>
     </row>
     <row r="86" spans="1:4" ht="18" customHeight="1">
       <c r="A86" s="24"/>
-      <c r="B86" s="63"/>
-      <c r="C86" s="64"/>
+      <c r="B86" s="49"/>
+      <c r="C86" s="50"/>
       <c r="D86" s="25"/>
     </row>
     <row r="87" spans="1:4" ht="18" customHeight="1">
       <c r="A87" s="24"/>
-      <c r="B87" s="63"/>
-      <c r="C87" s="64"/>
+      <c r="B87" s="49"/>
+      <c r="C87" s="50"/>
       <c r="D87" s="25"/>
     </row>
     <row r="88" spans="1:4" ht="18" customHeight="1">
       <c r="A88" s="24"/>
-      <c r="B88" s="63"/>
-      <c r="C88" s="64"/>
+      <c r="B88" s="49"/>
+      <c r="C88" s="50"/>
       <c r="D88" s="25"/>
     </row>
     <row r="89" spans="1:4" ht="18" customHeight="1">
       <c r="A89" s="24"/>
-      <c r="B89" s="63"/>
-      <c r="C89" s="64"/>
+      <c r="B89" s="49"/>
+      <c r="C89" s="50"/>
       <c r="D89" s="25"/>
     </row>
     <row r="90" spans="1:4" ht="18" customHeight="1">
       <c r="A90" s="24"/>
-      <c r="B90" s="63"/>
-      <c r="C90" s="64"/>
+      <c r="B90" s="49"/>
+      <c r="C90" s="50"/>
       <c r="D90" s="25"/>
     </row>
     <row r="91" spans="1:4" ht="18" customHeight="1">
       <c r="A91" s="24"/>
-      <c r="B91" s="63"/>
-      <c r="C91" s="64"/>
+      <c r="B91" s="49"/>
+      <c r="C91" s="50"/>
       <c r="D91" s="25"/>
     </row>
     <row r="92" spans="1:4" ht="18" customHeight="1">
       <c r="A92" s="24"/>
-      <c r="B92" s="63"/>
-      <c r="C92" s="64"/>
+      <c r="B92" s="49"/>
+      <c r="C92" s="50"/>
       <c r="D92" s="25"/>
     </row>
     <row r="93" spans="1:4" ht="18" customHeight="1">
       <c r="A93" s="24"/>
-      <c r="B93" s="63"/>
-      <c r="C93" s="64"/>
+      <c r="B93" s="49"/>
+      <c r="C93" s="50"/>
       <c r="D93" s="25"/>
     </row>
     <row r="94" spans="1:4" ht="18" customHeight="1">
       <c r="A94" s="24"/>
-      <c r="B94" s="63"/>
-      <c r="C94" s="64"/>
+      <c r="B94" s="49"/>
+      <c r="C94" s="50"/>
       <c r="D94" s="25"/>
     </row>
     <row r="95" spans="1:4" ht="18" customHeight="1">
       <c r="A95" s="24"/>
-      <c r="B95" s="63"/>
-      <c r="C95" s="64"/>
+      <c r="B95" s="49"/>
+      <c r="C95" s="50"/>
       <c r="D95" s="25"/>
     </row>
     <row r="96" spans="1:4" ht="18" customHeight="1">
       <c r="A96" s="24"/>
-      <c r="B96" s="63"/>
-      <c r="C96" s="64"/>
+      <c r="B96" s="49"/>
+      <c r="C96" s="50"/>
       <c r="D96" s="25"/>
     </row>
     <row r="97" spans="1:4" ht="18" customHeight="1">
       <c r="A97" s="24"/>
-      <c r="B97" s="63"/>
-      <c r="C97" s="64"/>
+      <c r="B97" s="49"/>
+      <c r="C97" s="50"/>
       <c r="D97" s="25"/>
     </row>
     <row r="98" spans="1:4" ht="18" customHeight="1">
       <c r="A98" s="24"/>
-      <c r="B98" s="63"/>
-      <c r="C98" s="64"/>
+      <c r="B98" s="49"/>
+      <c r="C98" s="50"/>
       <c r="D98" s="25"/>
     </row>
     <row r="99" spans="1:4" ht="18" customHeight="1">
       <c r="A99" s="24"/>
-      <c r="B99" s="63"/>
-      <c r="C99" s="64"/>
+      <c r="B99" s="49"/>
+      <c r="C99" s="50"/>
       <c r="D99" s="25"/>
     </row>
     <row r="100" spans="1:4" ht="18" customHeight="1">
       <c r="A100" s="24"/>
-      <c r="B100" s="63"/>
-      <c r="C100" s="64"/>
+      <c r="B100" s="49"/>
+      <c r="C100" s="50"/>
       <c r="D100" s="25"/>
     </row>
     <row r="101" spans="1:4" ht="18" customHeight="1">
       <c r="A101" s="24"/>
-      <c r="B101" s="63"/>
-      <c r="C101" s="64"/>
+      <c r="B101" s="49"/>
+      <c r="C101" s="50"/>
       <c r="D101" s="25"/>
     </row>
     <row r="102" spans="1:4" ht="18" customHeight="1">
       <c r="A102" s="24"/>
-      <c r="B102" s="63"/>
-      <c r="C102" s="64"/>
+      <c r="B102" s="49"/>
+      <c r="C102" s="50"/>
       <c r="D102" s="25"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="74">
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A40:G40"/>
     <mergeCell ref="B50:D50"/>
     <mergeCell ref="E46:F46"/>
     <mergeCell ref="E50:F50"/>
@@ -2835,15 +2801,55 @@
     <mergeCell ref="E44:F44"/>
     <mergeCell ref="B44:D44"/>
     <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B98:C98"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2883,497 +2889,497 @@
   <sheetData>
     <row r="1" spans="1:10" ht="22.5">
       <c r="A1" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1">
-      <c r="A3" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
+      <c r="A3" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1">
-      <c r="A4" s="65"/>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
+      <c r="A4" s="69"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="66"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="67"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="67"/>
-      <c r="J6" s="67"/>
+      <c r="A6" s="71"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="67"/>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
+      <c r="A7" s="71"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="67"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="67"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="67"/>
-      <c r="B9" s="67"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
+      <c r="A9" s="71"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="67"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="67"/>
-      <c r="B11" s="67"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="67"/>
-      <c r="B12" s="67"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="67"/>
+      <c r="A12" s="71"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="67"/>
-      <c r="B13" s="67"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
+      <c r="A13" s="71"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="71"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="67"/>
-      <c r="B14" s="67"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="67"/>
-      <c r="J14" s="67"/>
+      <c r="A14" s="71"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="71"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="67"/>
-      <c r="B15" s="67"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="67"/>
+      <c r="A15" s="71"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="71"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="67"/>
-      <c r="B16" s="67"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
+      <c r="A16" s="71"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="71"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="67"/>
-      <c r="B17" s="67"/>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
+      <c r="A17" s="71"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="67"/>
-      <c r="B18" s="67"/>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
+      <c r="A18" s="71"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="67"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="67"/>
-      <c r="I19" s="67"/>
-      <c r="J19" s="67"/>
+      <c r="A19" s="71"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="71"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="67"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="67"/>
-      <c r="H20" s="67"/>
-      <c r="I20" s="67"/>
-      <c r="J20" s="67"/>
+      <c r="A20" s="71"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="71"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="67"/>
-      <c r="B21" s="67"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="67"/>
+      <c r="A21" s="71"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="71"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="67"/>
-      <c r="B22" s="67"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="67"/>
-      <c r="J22" s="67"/>
+      <c r="A22" s="71"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="71"/>
+      <c r="J22" s="71"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="67"/>
-      <c r="B23" s="67"/>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="67"/>
-      <c r="H23" s="67"/>
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
+      <c r="A23" s="71"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="71"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="67"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
+      <c r="A24" s="71"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="67"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
-      <c r="H25" s="67"/>
-      <c r="I25" s="67"/>
-      <c r="J25" s="67"/>
+      <c r="A25" s="71"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="71"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="67"/>
-      <c r="B26" s="67"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="67"/>
-      <c r="H26" s="67"/>
-      <c r="I26" s="67"/>
-      <c r="J26" s="67"/>
+      <c r="A26" s="71"/>
+      <c r="B26" s="71"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="71"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="67"/>
-      <c r="B27" s="67"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="67"/>
-      <c r="G27" s="67"/>
-      <c r="H27" s="67"/>
-      <c r="I27" s="67"/>
-      <c r="J27" s="67"/>
+      <c r="A27" s="71"/>
+      <c r="B27" s="71"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="71"/>
+      <c r="J27" s="71"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="67"/>
-      <c r="B28" s="67"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="67"/>
-      <c r="F28" s="67"/>
-      <c r="G28" s="67"/>
-      <c r="H28" s="67"/>
-      <c r="I28" s="67"/>
-      <c r="J28" s="67"/>
+      <c r="A28" s="71"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="67"/>
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="67"/>
-      <c r="J29" s="67"/>
+      <c r="A29" s="71"/>
+      <c r="B29" s="71"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="71"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="71"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="71"/>
+      <c r="J29" s="71"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="67"/>
-      <c r="B30" s="67"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="67"/>
-      <c r="H30" s="67"/>
-      <c r="I30" s="67"/>
-      <c r="J30" s="67"/>
+      <c r="A30" s="71"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="67"/>
-      <c r="B31" s="67"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="67"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="67"/>
-      <c r="J31" s="67"/>
+      <c r="A31" s="71"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="71"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="71"/>
+      <c r="I31" s="71"/>
+      <c r="J31" s="71"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="67"/>
-      <c r="B32" s="67"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="67"/>
-      <c r="H32" s="67"/>
-      <c r="I32" s="67"/>
-      <c r="J32" s="67"/>
+      <c r="A32" s="71"/>
+      <c r="B32" s="71"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="71"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="67"/>
-      <c r="B33" s="67"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="67"/>
-      <c r="G33" s="67"/>
-      <c r="H33" s="67"/>
-      <c r="I33" s="67"/>
-      <c r="J33" s="67"/>
+      <c r="A33" s="71"/>
+      <c r="B33" s="71"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="71"/>
+      <c r="J33" s="71"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="67"/>
-      <c r="B34" s="67"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="67"/>
-      <c r="F34" s="67"/>
-      <c r="G34" s="67"/>
-      <c r="H34" s="67"/>
-      <c r="I34" s="67"/>
-      <c r="J34" s="67"/>
+      <c r="A34" s="71"/>
+      <c r="B34" s="71"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="71"/>
+      <c r="J34" s="71"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="67"/>
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="67"/>
-      <c r="I35" s="67"/>
-      <c r="J35" s="67"/>
+      <c r="A35" s="71"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="71"/>
+      <c r="J35" s="71"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="67"/>
-      <c r="B36" s="67"/>
-      <c r="C36" s="67"/>
-      <c r="D36" s="67"/>
-      <c r="E36" s="67"/>
-      <c r="F36" s="67"/>
-      <c r="G36" s="67"/>
-      <c r="H36" s="67"/>
-      <c r="I36" s="67"/>
-      <c r="J36" s="67"/>
+      <c r="A36" s="71"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="71"/>
+      <c r="E36" s="71"/>
+      <c r="F36" s="71"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="71"/>
+      <c r="I36" s="71"/>
+      <c r="J36" s="71"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="67"/>
-      <c r="B37" s="67"/>
-      <c r="C37" s="67"/>
-      <c r="D37" s="67"/>
-      <c r="E37" s="67"/>
-      <c r="F37" s="67"/>
-      <c r="G37" s="67"/>
-      <c r="H37" s="67"/>
-      <c r="I37" s="67"/>
-      <c r="J37" s="67"/>
+      <c r="A37" s="71"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="71"/>
+      <c r="E37" s="71"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="71"/>
+      <c r="I37" s="71"/>
+      <c r="J37" s="71"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="67"/>
-      <c r="B38" s="67"/>
-      <c r="C38" s="67"/>
-      <c r="D38" s="67"/>
-      <c r="E38" s="67"/>
-      <c r="F38" s="67"/>
-      <c r="G38" s="67"/>
-      <c r="H38" s="67"/>
-      <c r="I38" s="67"/>
-      <c r="J38" s="67"/>
+      <c r="A38" s="71"/>
+      <c r="B38" s="71"/>
+      <c r="C38" s="71"/>
+      <c r="D38" s="71"/>
+      <c r="E38" s="71"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="71"/>
+      <c r="I38" s="71"/>
+      <c r="J38" s="71"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="67"/>
-      <c r="B39" s="67"/>
-      <c r="C39" s="67"/>
-      <c r="D39" s="67"/>
-      <c r="E39" s="67"/>
-      <c r="F39" s="67"/>
-      <c r="G39" s="67"/>
-      <c r="H39" s="67"/>
-      <c r="I39" s="67"/>
-      <c r="J39" s="67"/>
+      <c r="A39" s="71"/>
+      <c r="B39" s="71"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="71"/>
+      <c r="F39" s="71"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="71"/>
+      <c r="I39" s="71"/>
+      <c r="J39" s="71"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="67"/>
-      <c r="B40" s="67"/>
-      <c r="C40" s="67"/>
-      <c r="D40" s="67"/>
-      <c r="E40" s="67"/>
-      <c r="F40" s="67"/>
-      <c r="G40" s="67"/>
-      <c r="H40" s="67"/>
-      <c r="I40" s="67"/>
-      <c r="J40" s="67"/>
+      <c r="A40" s="71"/>
+      <c r="B40" s="71"/>
+      <c r="C40" s="71"/>
+      <c r="D40" s="71"/>
+      <c r="E40" s="71"/>
+      <c r="F40" s="71"/>
+      <c r="G40" s="71"/>
+      <c r="H40" s="71"/>
+      <c r="I40" s="71"/>
+      <c r="J40" s="71"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="67"/>
-      <c r="B41" s="67"/>
-      <c r="C41" s="67"/>
-      <c r="D41" s="67"/>
-      <c r="E41" s="67"/>
-      <c r="F41" s="67"/>
-      <c r="G41" s="67"/>
-      <c r="H41" s="67"/>
-      <c r="I41" s="67"/>
-      <c r="J41" s="67"/>
+      <c r="A41" s="71"/>
+      <c r="B41" s="71"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="71"/>
+      <c r="F41" s="71"/>
+      <c r="G41" s="71"/>
+      <c r="H41" s="71"/>
+      <c r="I41" s="71"/>
+      <c r="J41" s="71"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="67"/>
-      <c r="B42" s="67"/>
-      <c r="C42" s="67"/>
-      <c r="D42" s="67"/>
-      <c r="E42" s="67"/>
-      <c r="F42" s="67"/>
-      <c r="G42" s="67"/>
-      <c r="H42" s="67"/>
-      <c r="I42" s="67"/>
-      <c r="J42" s="67"/>
+      <c r="A42" s="71"/>
+      <c r="B42" s="71"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
+      <c r="F42" s="71"/>
+      <c r="G42" s="71"/>
+      <c r="H42" s="71"/>
+      <c r="I42" s="71"/>
+      <c r="J42" s="71"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>0</v>
       </c>
       <c r="B43" s="40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C43" s="40"/>
       <c r="D43" s="40"/>
@@ -3402,76 +3408,76 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
   <sheetData>
     <row r="1" spans="1:9" ht="15">
-      <c r="A1" s="68" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
+      <c r="A1" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
     </row>
     <row r="2" spans="1:9" ht="20.25" thickBot="1">
       <c r="A2" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" t="s">
         <v>76</v>
-      </c>
-      <c r="I2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1">
       <c r="A3" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G3" s="26"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="A4" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G4" s="26"/>
     </row>
     <row r="5" spans="1:9" ht="17.25" customHeight="1" thickBot="1">
       <c r="A5" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G5" s="26"/>
       <c r="I5" s="26"/>
     </row>
     <row r="6" spans="1:9" ht="27" customHeight="1" thickBot="1">
-      <c r="A6" s="69" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
+      <c r="A6" s="73" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
       <c r="G6" s="26"/>
       <c r="I6" s="26"/>
     </row>
     <row r="8" spans="1:9" ht="20.25" thickBot="1">
       <c r="A8" s="29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1">
       <c r="A10" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
@@ -3480,86 +3486,86 @@
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1">
       <c r="A11" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G11" s="26"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G12" s="26"/>
     </row>
     <row r="14" spans="1:9" ht="20.25" thickBot="1">
       <c r="A14" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" t="s">
         <v>76</v>
-      </c>
-      <c r="I14" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1">
       <c r="A15" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G15" s="26"/>
       <c r="I15" s="26"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1">
       <c r="A16" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G16" s="26"/>
       <c r="I16" s="26"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G17" s="26"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1">
       <c r="A18" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G18" s="26"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1">
       <c r="A19" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G19" s="26"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1">
       <c r="A20" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G20" s="26"/>
       <c r="I20" s="26"/>
     </row>
     <row r="21" spans="1:9" ht="29.25" customHeight="1">
-      <c r="A21" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
+      <c r="A21" s="75" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" thickBot="1">
       <c r="A22" s="5"/>
     </row>
     <row r="23" spans="1:9" ht="46.5" customHeight="1" thickBot="1">
-      <c r="A23" s="72" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" s="73"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
+      <c r="A23" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="77"/>
+      <c r="C23" s="77"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="77"/>
       <c r="G23" s="26"/>
     </row>
     <row r="24" spans="1:9" ht="15">
@@ -3567,27 +3573,27 @@
     </row>
     <row r="25" spans="1:9" ht="15">
       <c r="A25" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15">
       <c r="A27" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15">
       <c r="A28" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="B30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E30" s="30"/>
     </row>

</xml_diff>

<commit_message>
20190206 Trick video load, Chief official contact validation, Slalom pass detail report
</commit_message>
<xml_diff>
--- a/WaterskiScoringSystem/WaterskiScoringSystem/RecordApplicationFormTemplate.xlsx
+++ b/WaterskiScoringSystem/WaterskiScoringSystem/RecordApplicationFormTemplate.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WaterskiScoring\GitHub\WaterskiScoringSystem\WaterskiScoringSystem\WaterskiScoringSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4AE6EF6-9445-4732-A631-4D991662EBE7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4725" yWindow="120" windowWidth="14670" windowHeight="7710" tabRatio="849" activeTab="1"/>
+    <workbookView xWindow="4728" yWindow="120" windowWidth="14676" windowHeight="7716" tabRatio="849" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COVER PAGE" sheetId="7" r:id="rId1"/>
@@ -78,9 +79,6 @@
     <t xml:space="preserve">Address: </t>
   </si>
   <si>
-    <t xml:space="preserve">Birth date: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Name: </t>
   </si>
   <si>
@@ -365,11 +363,14 @@
   <si>
     <t>Manufacture:</t>
   </si>
+  <si>
+    <t xml:space="preserve">Ski Year Age: </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
@@ -757,14 +758,6 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -794,6 +787,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1262,26 +1263,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A31" sqref="A31:M31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="11.4"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.375" customWidth="1"/>
+    <col min="2" max="2" width="4.125" customWidth="1"/>
+    <col min="10" max="10" width="10.125" customWidth="1"/>
+    <col min="11" max="11" width="12.125" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="26.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="24.6">
       <c r="A1" s="46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -1311,7 +1312,7 @@
       <c r="L2" s="40"/>
       <c r="M2" s="40"/>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" ht="18">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="17.399999999999999">
       <c r="A3" s="48" t="s">
         <v>5</v>
       </c>
@@ -1343,9 +1344,9 @@
       <c r="L4" s="40"/>
       <c r="M4" s="40"/>
     </row>
-    <row r="5" spans="1:13" ht="18">
+    <row r="5" spans="1:13" ht="17.399999999999999">
       <c r="A5" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
@@ -1375,9 +1376,9 @@
       <c r="L6" s="40"/>
       <c r="M6" s="40"/>
     </row>
-    <row r="7" spans="1:13" ht="15">
+    <row r="7" spans="1:13" ht="13.8">
       <c r="A7" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -1394,7 +1395,7 @@
     </row>
     <row r="8" spans="1:13" ht="48" customHeight="1">
       <c r="A8" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="38"/>
       <c r="C8" s="38"/>
@@ -1424,9 +1425,9 @@
       <c r="L9" s="37"/>
       <c r="M9" s="37"/>
     </row>
-    <row r="10" spans="1:13" ht="15">
+    <row r="10" spans="1:13" ht="13.8">
       <c r="A10" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="37"/>
       <c r="C10" s="37"/>
@@ -1443,7 +1444,7 @@
     </row>
     <row r="11" spans="1:13" ht="36" customHeight="1">
       <c r="A11" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
@@ -1473,9 +1474,9 @@
       <c r="L12" s="37"/>
       <c r="M12" s="37"/>
     </row>
-    <row r="13" spans="1:13" ht="15">
+    <row r="13" spans="1:13" ht="13.8">
       <c r="A13" s="39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="40"/>
@@ -1492,7 +1493,7 @@
     </row>
     <row r="14" spans="1:13" ht="24" customHeight="1">
       <c r="A14" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
@@ -1522,9 +1523,9 @@
       <c r="L15" s="37"/>
       <c r="M15" s="37"/>
     </row>
-    <row r="16" spans="1:13" ht="15">
+    <row r="16" spans="1:13" ht="13.8">
       <c r="A16" s="41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="40"/>
       <c r="C16" s="40"/>
@@ -1541,7 +1542,7 @@
     </row>
     <row r="17" spans="1:13" ht="24" customHeight="1">
       <c r="A17" s="38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
@@ -1556,7 +1557,7 @@
       <c r="L17" s="38"/>
       <c r="M17" s="38"/>
     </row>
-    <row r="18" spans="1:13" ht="15">
+    <row r="18" spans="1:13" ht="13.8">
       <c r="A18" s="41"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -1571,9 +1572,9 @@
       <c r="L18" s="37"/>
       <c r="M18" s="37"/>
     </row>
-    <row r="19" spans="1:13" ht="15">
+    <row r="19" spans="1:13" ht="13.8">
       <c r="A19" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="40"/>
       <c r="C19" s="40"/>
@@ -1590,7 +1591,7 @@
     </row>
     <row r="20" spans="1:13" ht="48" customHeight="1">
       <c r="A20" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
@@ -1620,9 +1621,9 @@
       <c r="L21" s="37"/>
       <c r="M21" s="37"/>
     </row>
-    <row r="22" spans="1:13" ht="15">
+    <row r="22" spans="1:13" ht="13.8">
       <c r="A22" s="42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" s="37"/>
       <c r="C22" s="37"/>
@@ -1639,7 +1640,7 @@
     </row>
     <row r="23" spans="1:13" ht="48" customHeight="1">
       <c r="A23" s="35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B23" s="36"/>
       <c r="C23" s="36"/>
@@ -1669,9 +1670,9 @@
       <c r="L24" s="37"/>
       <c r="M24" s="37"/>
     </row>
-    <row r="25" spans="1:13" ht="15">
+    <row r="25" spans="1:13" ht="13.8">
       <c r="A25" s="42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
@@ -1688,7 +1689,7 @@
     </row>
     <row r="26" spans="1:13" ht="60" customHeight="1">
       <c r="A26" s="35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -1718,9 +1719,9 @@
       <c r="L27" s="37"/>
       <c r="M27" s="37"/>
     </row>
-    <row r="28" spans="1:13" ht="15">
+    <row r="28" spans="1:13" ht="13.8">
       <c r="A28" s="42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" s="37"/>
       <c r="C28" s="37"/>
@@ -1737,7 +1738,7 @@
     </row>
     <row r="29" spans="1:13" ht="36" customHeight="1">
       <c r="A29" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B29" s="36"/>
       <c r="C29" s="36"/>
@@ -1769,7 +1770,7 @@
     </row>
     <row r="31" spans="1:13" ht="60" customHeight="1">
       <c r="A31" s="43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B31" s="44"/>
       <c r="C31" s="44"/>
@@ -1799,9 +1800,9 @@
       <c r="L32" s="37"/>
       <c r="M32" s="37"/>
     </row>
-    <row r="33" spans="1:13" ht="15">
+    <row r="33" spans="1:13" ht="13.8">
       <c r="A33" s="39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B33" s="37"/>
       <c r="C33" s="37"/>
@@ -1818,7 +1819,7 @@
     </row>
     <row r="34" spans="1:13" ht="108" customHeight="1">
       <c r="A34" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" s="38"/>
       <c r="C34" s="38"/>
@@ -1848,9 +1849,9 @@
       <c r="L35" s="37"/>
       <c r="M35" s="37"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" ht="12">
       <c r="A36" s="45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B36" s="45"/>
       <c r="C36" s="45"/>
@@ -1912,26 +1913,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34:G34"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="11.4"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.75" style="1" customWidth="1"/>
+    <col min="3" max="4" width="12.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.85546875" style="1"/>
+    <col min="8" max="8" width="19.625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1">
@@ -1939,21 +1940,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="26.25">
+    <row r="2" spans="1:8" ht="24.6">
       <c r="B2" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:8" ht="18" customHeight="1"/>
     <row r="4" spans="1:8" ht="18" customHeight="1">
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1964,7 +1965,7 @@
     </row>
     <row r="6" spans="1:8" ht="15">
       <c r="A6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -1975,7 +1976,7 @@
     </row>
     <row r="7" spans="1:8" ht="15">
       <c r="A7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -1996,7 +1997,7 @@
     </row>
     <row r="9" spans="1:8" ht="15">
       <c r="A9" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
@@ -2007,7 +2008,7 @@
     </row>
     <row r="10" spans="1:8" ht="15">
       <c r="A10" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="4"/>
       <c r="D10" s="5"/>
@@ -2026,7 +2027,7 @@
     </row>
     <row r="12" spans="1:8" ht="18" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -2128,7 +2129,7 @@
     </row>
     <row r="22" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A22" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2139,13 +2140,13 @@
     </row>
     <row r="23" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A23" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="54"/>
       <c r="C23" s="63"/>
       <c r="D23" s="55"/>
       <c r="E23" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F23" s="54"/>
       <c r="G23" s="55"/>
@@ -2161,7 +2162,7 @@
     </row>
     <row r="25" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A25" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="58"/>
       <c r="C25" s="59"/>
@@ -2187,10 +2188,10 @@
       <c r="C27" s="59"/>
       <c r="D27" s="60"/>
       <c r="E27" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="66"/>
-      <c r="G27" s="67"/>
+        <v>100</v>
+      </c>
+      <c r="F27" s="77"/>
+      <c r="G27" s="76"/>
     </row>
     <row r="28" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A28" s="5"/>
@@ -2203,7 +2204,7 @@
     </row>
     <row r="29" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A29" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29" s="54"/>
       <c r="C29" s="63"/>
@@ -2223,7 +2224,7 @@
     </row>
     <row r="31" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A31" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="27"/>
       <c r="C31" s="27"/>
@@ -2243,38 +2244,38 @@
     </row>
     <row r="33" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A33" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
       <c r="E33" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A34" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34" s="61"/>
       <c r="C34" s="62"/>
       <c r="D34" s="13"/>
       <c r="E34" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F34" s="54"/>
       <c r="G34" s="55"/>
     </row>
     <row r="35" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A35" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="61"/>
       <c r="C35" s="62"/>
       <c r="D35" s="13"/>
       <c r="E35" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="16"/>
@@ -2299,8 +2300,8 @@
       <c r="G37" s="5"/>
     </row>
     <row r="38" spans="1:8" ht="18" customHeight="1">
-      <c r="A38" s="68" t="s">
-        <v>99</v>
+      <c r="A38" s="66" t="s">
+        <v>98</v>
       </c>
       <c r="B38" s="40"/>
       <c r="C38" s="40"/>
@@ -2310,8 +2311,8 @@
       <c r="G38" s="40"/>
     </row>
     <row r="39" spans="1:8" ht="18" customHeight="1">
-      <c r="A39" s="68" t="s">
-        <v>49</v>
+      <c r="A39" s="66" t="s">
+        <v>48</v>
       </c>
       <c r="B39" s="40"/>
       <c r="C39" s="40"/>
@@ -2321,8 +2322,8 @@
       <c r="G39" s="40"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1">
-      <c r="A40" s="68" t="s">
-        <v>51</v>
+      <c r="A40" s="66" t="s">
+        <v>50</v>
       </c>
       <c r="B40" s="40"/>
       <c r="C40" s="40"/>
@@ -2341,7 +2342,7 @@
     </row>
     <row r="42" spans="1:8" ht="18" customHeight="1">
       <c r="A42" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -2355,13 +2356,13 @@
         <v>2</v>
       </c>
       <c r="B43" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G43" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="H43" s="9" t="s">
         <v>4</v>
@@ -2369,7 +2370,7 @@
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A44" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B44" s="51"/>
       <c r="C44" s="51"/>
@@ -2391,7 +2392,7 @@
     </row>
     <row r="46" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A46" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B46" s="51"/>
       <c r="C46" s="51"/>
@@ -2404,7 +2405,7 @@
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A47" s="5"/>
       <c r="B47" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -2415,7 +2416,7 @@
     </row>
     <row r="48" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A48" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48" s="51"/>
       <c r="C48" s="51"/>
@@ -2437,7 +2438,7 @@
     </row>
     <row r="50" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A50" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B50" s="51"/>
       <c r="C50" s="51"/>
@@ -2472,7 +2473,7 @@
     <row r="53" spans="1:8" ht="18" customHeight="1">
       <c r="A53" s="3"/>
       <c r="B53" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="6" t="s">
@@ -2775,7 +2776,7 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="74">
+  <mergeCells count="73">
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="E48:F48"/>
@@ -2797,7 +2798,6 @@
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F27:G27"/>
     <mergeCell ref="E44:F44"/>
     <mergeCell ref="B44:D44"/>
     <mergeCell ref="B29:F29"/>
@@ -2861,14 +2861,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="33"/>
+    <col min="1" max="16384" width="9.125" style="33"/>
   </cols>
   <sheetData>
     <row r="1" s="34" customFormat="1"/>
@@ -2878,508 +2878,508 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B43" sqref="B43:D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="11.4"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="22.5">
+    <row r="1" spans="1:10" ht="21">
       <c r="A1" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1">
-      <c r="A3" s="69" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
+      <c r="A3" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1">
-      <c r="A4" s="69"/>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
+      <c r="A4" s="67"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="70"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
+      <c r="A5" s="68"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="71"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
+      <c r="A6" s="69"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="71"/>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
+      <c r="A7" s="69"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="71"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
+      <c r="A8" s="69"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="71"/>
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="71"/>
+      <c r="A9" s="69"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="71"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="71"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="71"/>
+      <c r="A10" s="69"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="71"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="71"/>
+      <c r="A11" s="69"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="69"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="71"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
+      <c r="A12" s="69"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="71"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="71"/>
+      <c r="A13" s="69"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="71"/>
-      <c r="B14" s="71"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="71"/>
-      <c r="H14" s="71"/>
-      <c r="I14" s="71"/>
-      <c r="J14" s="71"/>
+      <c r="A14" s="69"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="69"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="71"/>
-      <c r="B15" s="71"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="71"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="71"/>
+      <c r="A15" s="69"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="71"/>
-      <c r="B16" s="71"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
-      <c r="H16" s="71"/>
-      <c r="I16" s="71"/>
-      <c r="J16" s="71"/>
+      <c r="A16" s="69"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="71"/>
-      <c r="B17" s="71"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="71"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="71"/>
+      <c r="A17" s="69"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="69"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="71"/>
-      <c r="B18" s="71"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
+      <c r="A18" s="69"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="71"/>
-      <c r="B19" s="71"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="71"/>
-      <c r="I19" s="71"/>
-      <c r="J19" s="71"/>
+      <c r="A19" s="69"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="71"/>
-      <c r="B20" s="71"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="71"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="71"/>
+      <c r="A20" s="69"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="69"/>
+      <c r="J20" s="69"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="71"/>
-      <c r="B21" s="71"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="71"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="71"/>
+      <c r="A21" s="69"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="69"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="71"/>
-      <c r="B22" s="71"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="71"/>
-      <c r="I22" s="71"/>
-      <c r="J22" s="71"/>
+      <c r="A22" s="69"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="69"/>
+      <c r="J22" s="69"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="71"/>
-      <c r="B23" s="71"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="71"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="71"/>
+      <c r="A23" s="69"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="69"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="69"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="71"/>
-      <c r="B24" s="71"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
+      <c r="A24" s="69"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="71"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="71"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="71"/>
+      <c r="A25" s="69"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="69"/>
+      <c r="I25" s="69"/>
+      <c r="J25" s="69"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="71"/>
-      <c r="B26" s="71"/>
-      <c r="C26" s="71"/>
-      <c r="D26" s="71"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="71"/>
+      <c r="A26" s="69"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="69"/>
+      <c r="I26" s="69"/>
+      <c r="J26" s="69"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="71"/>
-      <c r="B27" s="71"/>
-      <c r="C27" s="71"/>
-      <c r="D27" s="71"/>
-      <c r="E27" s="71"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="71"/>
-      <c r="I27" s="71"/>
-      <c r="J27" s="71"/>
+      <c r="A27" s="69"/>
+      <c r="B27" s="69"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
+      <c r="G27" s="69"/>
+      <c r="H27" s="69"/>
+      <c r="I27" s="69"/>
+      <c r="J27" s="69"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="71"/>
-      <c r="B28" s="71"/>
-      <c r="C28" s="71"/>
-      <c r="D28" s="71"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
+      <c r="A28" s="69"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="69"/>
+      <c r="I28" s="69"/>
+      <c r="J28" s="69"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="71"/>
-      <c r="B29" s="71"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="71"/>
-      <c r="E29" s="71"/>
-      <c r="F29" s="71"/>
-      <c r="G29" s="71"/>
-      <c r="H29" s="71"/>
-      <c r="I29" s="71"/>
-      <c r="J29" s="71"/>
+      <c r="A29" s="69"/>
+      <c r="B29" s="69"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="69"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="69"/>
+      <c r="I29" s="69"/>
+      <c r="J29" s="69"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="71"/>
-      <c r="B30" s="71"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="71"/>
+      <c r="A30" s="69"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="69"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="71"/>
-      <c r="B31" s="71"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="71"/>
-      <c r="E31" s="71"/>
-      <c r="F31" s="71"/>
-      <c r="G31" s="71"/>
-      <c r="H31" s="71"/>
-      <c r="I31" s="71"/>
-      <c r="J31" s="71"/>
+      <c r="A31" s="69"/>
+      <c r="B31" s="69"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="69"/>
+      <c r="I31" s="69"/>
+      <c r="J31" s="69"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="71"/>
-      <c r="B32" s="71"/>
-      <c r="C32" s="71"/>
-      <c r="D32" s="71"/>
-      <c r="E32" s="71"/>
-      <c r="F32" s="71"/>
-      <c r="G32" s="71"/>
-      <c r="H32" s="71"/>
-      <c r="I32" s="71"/>
-      <c r="J32" s="71"/>
+      <c r="A32" s="69"/>
+      <c r="B32" s="69"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="69"/>
+      <c r="G32" s="69"/>
+      <c r="H32" s="69"/>
+      <c r="I32" s="69"/>
+      <c r="J32" s="69"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="71"/>
-      <c r="B33" s="71"/>
-      <c r="C33" s="71"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="71"/>
-      <c r="G33" s="71"/>
-      <c r="H33" s="71"/>
-      <c r="I33" s="71"/>
-      <c r="J33" s="71"/>
+      <c r="A33" s="69"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="69"/>
+      <c r="J33" s="69"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="71"/>
-      <c r="B34" s="71"/>
-      <c r="C34" s="71"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="71"/>
-      <c r="F34" s="71"/>
-      <c r="G34" s="71"/>
-      <c r="H34" s="71"/>
-      <c r="I34" s="71"/>
-      <c r="J34" s="71"/>
+      <c r="A34" s="69"/>
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
+      <c r="J34" s="69"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="71"/>
-      <c r="B35" s="71"/>
-      <c r="C35" s="71"/>
-      <c r="D35" s="71"/>
-      <c r="E35" s="71"/>
-      <c r="F35" s="71"/>
-      <c r="G35" s="71"/>
-      <c r="H35" s="71"/>
-      <c r="I35" s="71"/>
-      <c r="J35" s="71"/>
+      <c r="A35" s="69"/>
+      <c r="B35" s="69"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="69"/>
+      <c r="J35" s="69"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="71"/>
-      <c r="B36" s="71"/>
-      <c r="C36" s="71"/>
-      <c r="D36" s="71"/>
-      <c r="E36" s="71"/>
-      <c r="F36" s="71"/>
-      <c r="G36" s="71"/>
-      <c r="H36" s="71"/>
-      <c r="I36" s="71"/>
-      <c r="J36" s="71"/>
+      <c r="A36" s="69"/>
+      <c r="B36" s="69"/>
+      <c r="C36" s="69"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="69"/>
+      <c r="H36" s="69"/>
+      <c r="I36" s="69"/>
+      <c r="J36" s="69"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="71"/>
-      <c r="B37" s="71"/>
-      <c r="C37" s="71"/>
-      <c r="D37" s="71"/>
-      <c r="E37" s="71"/>
-      <c r="F37" s="71"/>
-      <c r="G37" s="71"/>
-      <c r="H37" s="71"/>
-      <c r="I37" s="71"/>
-      <c r="J37" s="71"/>
+      <c r="A37" s="69"/>
+      <c r="B37" s="69"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="69"/>
+      <c r="H37" s="69"/>
+      <c r="I37" s="69"/>
+      <c r="J37" s="69"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="71"/>
-      <c r="B38" s="71"/>
-      <c r="C38" s="71"/>
-      <c r="D38" s="71"/>
-      <c r="E38" s="71"/>
-      <c r="F38" s="71"/>
-      <c r="G38" s="71"/>
-      <c r="H38" s="71"/>
-      <c r="I38" s="71"/>
-      <c r="J38" s="71"/>
+      <c r="A38" s="69"/>
+      <c r="B38" s="69"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="69"/>
+      <c r="G38" s="69"/>
+      <c r="H38" s="69"/>
+      <c r="I38" s="69"/>
+      <c r="J38" s="69"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="71"/>
-      <c r="B39" s="71"/>
-      <c r="C39" s="71"/>
-      <c r="D39" s="71"/>
-      <c r="E39" s="71"/>
-      <c r="F39" s="71"/>
-      <c r="G39" s="71"/>
-      <c r="H39" s="71"/>
-      <c r="I39" s="71"/>
-      <c r="J39" s="71"/>
+      <c r="A39" s="69"/>
+      <c r="B39" s="69"/>
+      <c r="C39" s="69"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="69"/>
+      <c r="I39" s="69"/>
+      <c r="J39" s="69"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="71"/>
-      <c r="B40" s="71"/>
-      <c r="C40" s="71"/>
-      <c r="D40" s="71"/>
-      <c r="E40" s="71"/>
-      <c r="F40" s="71"/>
-      <c r="G40" s="71"/>
-      <c r="H40" s="71"/>
-      <c r="I40" s="71"/>
-      <c r="J40" s="71"/>
+      <c r="A40" s="69"/>
+      <c r="B40" s="69"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="69"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="69"/>
+      <c r="G40" s="69"/>
+      <c r="H40" s="69"/>
+      <c r="I40" s="69"/>
+      <c r="J40" s="69"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="71"/>
-      <c r="B41" s="71"/>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
-      <c r="E41" s="71"/>
-      <c r="F41" s="71"/>
-      <c r="G41" s="71"/>
-      <c r="H41" s="71"/>
-      <c r="I41" s="71"/>
-      <c r="J41" s="71"/>
+      <c r="A41" s="69"/>
+      <c r="B41" s="69"/>
+      <c r="C41" s="69"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="69"/>
+      <c r="G41" s="69"/>
+      <c r="H41" s="69"/>
+      <c r="I41" s="69"/>
+      <c r="J41" s="69"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="71"/>
-      <c r="B42" s="71"/>
-      <c r="C42" s="71"/>
-      <c r="D42" s="71"/>
-      <c r="E42" s="71"/>
-      <c r="F42" s="71"/>
-      <c r="G42" s="71"/>
-      <c r="H42" s="71"/>
-      <c r="I42" s="71"/>
-      <c r="J42" s="71"/>
+      <c r="A42" s="69"/>
+      <c r="B42" s="69"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="69"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="69"/>
+      <c r="I42" s="69"/>
+      <c r="J42" s="69"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>0</v>
       </c>
       <c r="B43" s="40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" s="40"/>
       <c r="D43" s="40"/>
@@ -3398,18 +3398,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="11.4"/>
   <sheetData>
     <row r="1" spans="1:9" ht="15">
-      <c r="A1" s="72" t="s">
-        <v>73</v>
+      <c r="A1" s="70" t="s">
+        <v>72</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -3420,152 +3420,152 @@
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
     </row>
-    <row r="2" spans="1:9" ht="20.25" thickBot="1">
+    <row r="2" spans="1:9" ht="19.2" thickBot="1">
       <c r="A2" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" t="s">
         <v>75</v>
       </c>
-      <c r="I2" t="s">
+    </row>
+    <row r="3" spans="1:9" ht="15.6" thickBot="1">
+      <c r="A3" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A3" s="5" t="s">
+      <c r="G3" s="26"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.6" thickBot="1">
+      <c r="A4" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="G3" s="26"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A4" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="G4" s="26"/>
     </row>
     <row r="5" spans="1:9" ht="17.25" customHeight="1" thickBot="1">
       <c r="A5" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G5" s="26"/>
       <c r="I5" s="26"/>
     </row>
     <row r="6" spans="1:9" ht="27" customHeight="1" thickBot="1">
-      <c r="A6" s="73" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="74"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
+      <c r="A6" s="71" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
       <c r="G6" s="26"/>
       <c r="I6" s="26"/>
     </row>
-    <row r="8" spans="1:9" ht="20.25" thickBot="1">
+    <row r="8" spans="1:9" ht="19.2" thickBot="1">
       <c r="A8" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.6" thickBot="1">
+      <c r="A9" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A9" s="5" t="s">
+      <c r="G9" s="26"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.6" thickBot="1">
+      <c r="A10" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="G9" s="26"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A10" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
       </c>
       <c r="G10" s="26"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+    <row r="11" spans="1:9" ht="15.6" thickBot="1">
       <c r="A11" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.6" thickBot="1">
+      <c r="A12" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G11" s="26"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A12" s="5" t="s">
+      <c r="G12" s="26"/>
+    </row>
+    <row r="14" spans="1:9" ht="19.2" thickBot="1">
+      <c r="A14" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="G12" s="26"/>
-    </row>
-    <row r="14" spans="1:9" ht="20.25" thickBot="1">
-      <c r="A14" s="29" t="s">
-        <v>86</v>
-      </c>
       <c r="G14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" t="s">
         <v>75</v>
       </c>
-      <c r="I14" t="s">
+    </row>
+    <row r="15" spans="1:9" ht="15.6" thickBot="1">
+      <c r="A15" s="5" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A15" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="G15" s="26"/>
       <c r="I15" s="26"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1">
+    <row r="16" spans="1:9" ht="15.6" thickBot="1">
       <c r="A16" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G16" s="26"/>
       <c r="I16" s="26"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1">
+    <row r="17" spans="1:9" ht="15.6" thickBot="1">
       <c r="A17" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" s="26"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.6" thickBot="1">
+      <c r="A18" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="26"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A18" s="5" t="s">
+      <c r="G18" s="26"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.6" thickBot="1">
+      <c r="A19" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="G18" s="26"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A19" s="5" t="s">
+      <c r="G19" s="26"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.6" thickBot="1">
+      <c r="A20" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="G19" s="26"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A20" s="5" t="s">
-        <v>91</v>
       </c>
       <c r="G20" s="26"/>
       <c r="I20" s="26"/>
     </row>
     <row r="21" spans="1:9" ht="29.25" customHeight="1">
-      <c r="A21" s="75" t="s">
-        <v>92</v>
+      <c r="A21" s="73" t="s">
+        <v>91</v>
       </c>
       <c r="B21" s="38"/>
       <c r="C21" s="38"/>
       <c r="D21" s="38"/>
       <c r="E21" s="38"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1">
+    <row r="22" spans="1:9" ht="15.6" thickBot="1">
       <c r="A22" s="5"/>
     </row>
     <row r="23" spans="1:9" ht="46.5" customHeight="1" thickBot="1">
-      <c r="A23" s="76" t="s">
-        <v>93</v>
-      </c>
-      <c r="B23" s="77"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
+      <c r="A23" s="74" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
       <c r="G23" s="26"/>
     </row>
     <row r="24" spans="1:9" ht="15">
@@ -3573,27 +3573,27 @@
     </row>
     <row r="25" spans="1:9" ht="15">
       <c r="A25" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15">
       <c r="A27" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15">
       <c r="A28" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="B30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E30" s="30"/>
     </row>

</xml_diff>

<commit_message>
Feature/v5.0.1.3 Released 4/9/2019 (#24)
* v5.0.1.3 Updated 11/11/2018

* v5.0.1.3 Phase 1 commit.  Primary update was refactoring to slalom score calculation to better handle ZBS

* 20190206 Trick video load, Chief official contact validation, Slalom pass detail report

* 5.0.1.3 Released 4/9/2019 See Release notes for details
</commit_message>
<xml_diff>
--- a/WaterskiScoringSystem/WaterskiScoringSystem/RecordApplicationFormTemplate.xlsx
+++ b/WaterskiScoringSystem/WaterskiScoringSystem/RecordApplicationFormTemplate.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WaterskiScoring\GitHub\WaterskiScoringSystem\WaterskiScoringSystem\WaterskiScoringSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4AE6EF6-9445-4732-A631-4D991662EBE7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4725" yWindow="120" windowWidth="14670" windowHeight="7710" tabRatio="849" activeTab="1"/>
+    <workbookView xWindow="4728" yWindow="120" windowWidth="14676" windowHeight="7716" tabRatio="849" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COVER PAGE" sheetId="7" r:id="rId1"/>
@@ -78,9 +79,6 @@
     <t xml:space="preserve">Address: </t>
   </si>
   <si>
-    <t xml:space="preserve">Birth date: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Name: </t>
   </si>
   <si>
@@ -365,11 +363,14 @@
   <si>
     <t>Manufacture:</t>
   </si>
+  <si>
+    <t xml:space="preserve">Ski Year Age: </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
@@ -757,14 +758,6 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -794,6 +787,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1262,26 +1263,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A31" sqref="A31:M31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="11.4"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.375" customWidth="1"/>
+    <col min="2" max="2" width="4.125" customWidth="1"/>
+    <col min="10" max="10" width="10.125" customWidth="1"/>
+    <col min="11" max="11" width="12.125" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="26.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="24.6">
       <c r="A1" s="46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -1311,7 +1312,7 @@
       <c r="L2" s="40"/>
       <c r="M2" s="40"/>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" ht="18">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="17.399999999999999">
       <c r="A3" s="48" t="s">
         <v>5</v>
       </c>
@@ -1343,9 +1344,9 @@
       <c r="L4" s="40"/>
       <c r="M4" s="40"/>
     </row>
-    <row r="5" spans="1:13" ht="18">
+    <row r="5" spans="1:13" ht="17.399999999999999">
       <c r="A5" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
@@ -1375,9 +1376,9 @@
       <c r="L6" s="40"/>
       <c r="M6" s="40"/>
     </row>
-    <row r="7" spans="1:13" ht="15">
+    <row r="7" spans="1:13" ht="13.8">
       <c r="A7" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
@@ -1394,7 +1395,7 @@
     </row>
     <row r="8" spans="1:13" ht="48" customHeight="1">
       <c r="A8" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="38"/>
       <c r="C8" s="38"/>
@@ -1424,9 +1425,9 @@
       <c r="L9" s="37"/>
       <c r="M9" s="37"/>
     </row>
-    <row r="10" spans="1:13" ht="15">
+    <row r="10" spans="1:13" ht="13.8">
       <c r="A10" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="37"/>
       <c r="C10" s="37"/>
@@ -1443,7 +1444,7 @@
     </row>
     <row r="11" spans="1:13" ht="36" customHeight="1">
       <c r="A11" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
@@ -1473,9 +1474,9 @@
       <c r="L12" s="37"/>
       <c r="M12" s="37"/>
     </row>
-    <row r="13" spans="1:13" ht="15">
+    <row r="13" spans="1:13" ht="13.8">
       <c r="A13" s="39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="40"/>
@@ -1492,7 +1493,7 @@
     </row>
     <row r="14" spans="1:13" ht="24" customHeight="1">
       <c r="A14" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
@@ -1522,9 +1523,9 @@
       <c r="L15" s="37"/>
       <c r="M15" s="37"/>
     </row>
-    <row r="16" spans="1:13" ht="15">
+    <row r="16" spans="1:13" ht="13.8">
       <c r="A16" s="41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="40"/>
       <c r="C16" s="40"/>
@@ -1541,7 +1542,7 @@
     </row>
     <row r="17" spans="1:13" ht="24" customHeight="1">
       <c r="A17" s="38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
@@ -1556,7 +1557,7 @@
       <c r="L17" s="38"/>
       <c r="M17" s="38"/>
     </row>
-    <row r="18" spans="1:13" ht="15">
+    <row r="18" spans="1:13" ht="13.8">
       <c r="A18" s="41"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -1571,9 +1572,9 @@
       <c r="L18" s="37"/>
       <c r="M18" s="37"/>
     </row>
-    <row r="19" spans="1:13" ht="15">
+    <row r="19" spans="1:13" ht="13.8">
       <c r="A19" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="40"/>
       <c r="C19" s="40"/>
@@ -1590,7 +1591,7 @@
     </row>
     <row r="20" spans="1:13" ht="48" customHeight="1">
       <c r="A20" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
@@ -1620,9 +1621,9 @@
       <c r="L21" s="37"/>
       <c r="M21" s="37"/>
     </row>
-    <row r="22" spans="1:13" ht="15">
+    <row r="22" spans="1:13" ht="13.8">
       <c r="A22" s="42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" s="37"/>
       <c r="C22" s="37"/>
@@ -1639,7 +1640,7 @@
     </row>
     <row r="23" spans="1:13" ht="48" customHeight="1">
       <c r="A23" s="35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B23" s="36"/>
       <c r="C23" s="36"/>
@@ -1669,9 +1670,9 @@
       <c r="L24" s="37"/>
       <c r="M24" s="37"/>
     </row>
-    <row r="25" spans="1:13" ht="15">
+    <row r="25" spans="1:13" ht="13.8">
       <c r="A25" s="42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
@@ -1688,7 +1689,7 @@
     </row>
     <row r="26" spans="1:13" ht="60" customHeight="1">
       <c r="A26" s="35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -1718,9 +1719,9 @@
       <c r="L27" s="37"/>
       <c r="M27" s="37"/>
     </row>
-    <row r="28" spans="1:13" ht="15">
+    <row r="28" spans="1:13" ht="13.8">
       <c r="A28" s="42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" s="37"/>
       <c r="C28" s="37"/>
@@ -1737,7 +1738,7 @@
     </row>
     <row r="29" spans="1:13" ht="36" customHeight="1">
       <c r="A29" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B29" s="36"/>
       <c r="C29" s="36"/>
@@ -1769,7 +1770,7 @@
     </row>
     <row r="31" spans="1:13" ht="60" customHeight="1">
       <c r="A31" s="43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B31" s="44"/>
       <c r="C31" s="44"/>
@@ -1799,9 +1800,9 @@
       <c r="L32" s="37"/>
       <c r="M32" s="37"/>
     </row>
-    <row r="33" spans="1:13" ht="15">
+    <row r="33" spans="1:13" ht="13.8">
       <c r="A33" s="39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B33" s="37"/>
       <c r="C33" s="37"/>
@@ -1818,7 +1819,7 @@
     </row>
     <row r="34" spans="1:13" ht="108" customHeight="1">
       <c r="A34" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" s="38"/>
       <c r="C34" s="38"/>
@@ -1848,9 +1849,9 @@
       <c r="L35" s="37"/>
       <c r="M35" s="37"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" ht="12">
       <c r="A36" s="45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B36" s="45"/>
       <c r="C36" s="45"/>
@@ -1912,26 +1913,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34:G34"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="11.4"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.75" style="1" customWidth="1"/>
+    <col min="3" max="4" width="12.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.85546875" style="1"/>
+    <col min="8" max="8" width="19.625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1">
@@ -1939,21 +1940,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="26.25">
+    <row r="2" spans="1:8" ht="24.6">
       <c r="B2" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:8" ht="18" customHeight="1"/>
     <row r="4" spans="1:8" ht="18" customHeight="1">
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1964,7 +1965,7 @@
     </row>
     <row r="6" spans="1:8" ht="15">
       <c r="A6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -1975,7 +1976,7 @@
     </row>
     <row r="7" spans="1:8" ht="15">
       <c r="A7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
@@ -1996,7 +1997,7 @@
     </row>
     <row r="9" spans="1:8" ht="15">
       <c r="A9" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
@@ -2007,7 +2008,7 @@
     </row>
     <row r="10" spans="1:8" ht="15">
       <c r="A10" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="4"/>
       <c r="D10" s="5"/>
@@ -2026,7 +2027,7 @@
     </row>
     <row r="12" spans="1:8" ht="18" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -2128,7 +2129,7 @@
     </row>
     <row r="22" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A22" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2139,13 +2140,13 @@
     </row>
     <row r="23" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A23" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="54"/>
       <c r="C23" s="63"/>
       <c r="D23" s="55"/>
       <c r="E23" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F23" s="54"/>
       <c r="G23" s="55"/>
@@ -2161,7 +2162,7 @@
     </row>
     <row r="25" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A25" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="58"/>
       <c r="C25" s="59"/>
@@ -2187,10 +2188,10 @@
       <c r="C27" s="59"/>
       <c r="D27" s="60"/>
       <c r="E27" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="66"/>
-      <c r="G27" s="67"/>
+        <v>100</v>
+      </c>
+      <c r="F27" s="77"/>
+      <c r="G27" s="76"/>
     </row>
     <row r="28" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A28" s="5"/>
@@ -2203,7 +2204,7 @@
     </row>
     <row r="29" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A29" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29" s="54"/>
       <c r="C29" s="63"/>
@@ -2223,7 +2224,7 @@
     </row>
     <row r="31" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A31" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="27"/>
       <c r="C31" s="27"/>
@@ -2243,38 +2244,38 @@
     </row>
     <row r="33" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A33" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
       <c r="E33" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A34" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34" s="61"/>
       <c r="C34" s="62"/>
       <c r="D34" s="13"/>
       <c r="E34" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F34" s="54"/>
       <c r="G34" s="55"/>
     </row>
     <row r="35" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A35" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="61"/>
       <c r="C35" s="62"/>
       <c r="D35" s="13"/>
       <c r="E35" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="16"/>
@@ -2299,8 +2300,8 @@
       <c r="G37" s="5"/>
     </row>
     <row r="38" spans="1:8" ht="18" customHeight="1">
-      <c r="A38" s="68" t="s">
-        <v>99</v>
+      <c r="A38" s="66" t="s">
+        <v>98</v>
       </c>
       <c r="B38" s="40"/>
       <c r="C38" s="40"/>
@@ -2310,8 +2311,8 @@
       <c r="G38" s="40"/>
     </row>
     <row r="39" spans="1:8" ht="18" customHeight="1">
-      <c r="A39" s="68" t="s">
-        <v>49</v>
+      <c r="A39" s="66" t="s">
+        <v>48</v>
       </c>
       <c r="B39" s="40"/>
       <c r="C39" s="40"/>
@@ -2321,8 +2322,8 @@
       <c r="G39" s="40"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1">
-      <c r="A40" s="68" t="s">
-        <v>51</v>
+      <c r="A40" s="66" t="s">
+        <v>50</v>
       </c>
       <c r="B40" s="40"/>
       <c r="C40" s="40"/>
@@ -2341,7 +2342,7 @@
     </row>
     <row r="42" spans="1:8" ht="18" customHeight="1">
       <c r="A42" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -2355,13 +2356,13 @@
         <v>2</v>
       </c>
       <c r="B43" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G43" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="H43" s="9" t="s">
         <v>4</v>
@@ -2369,7 +2370,7 @@
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A44" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B44" s="51"/>
       <c r="C44" s="51"/>
@@ -2391,7 +2392,7 @@
     </row>
     <row r="46" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A46" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B46" s="51"/>
       <c r="C46" s="51"/>
@@ -2404,7 +2405,7 @@
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A47" s="5"/>
       <c r="B47" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -2415,7 +2416,7 @@
     </row>
     <row r="48" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A48" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48" s="51"/>
       <c r="C48" s="51"/>
@@ -2437,7 +2438,7 @@
     </row>
     <row r="50" spans="1:8" ht="18" customHeight="1" thickBot="1">
       <c r="A50" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B50" s="51"/>
       <c r="C50" s="51"/>
@@ -2472,7 +2473,7 @@
     <row r="53" spans="1:8" ht="18" customHeight="1">
       <c r="A53" s="3"/>
       <c r="B53" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="6" t="s">
@@ -2775,7 +2776,7 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="74">
+  <mergeCells count="73">
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="E48:F48"/>
@@ -2797,7 +2798,6 @@
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F27:G27"/>
     <mergeCell ref="E44:F44"/>
     <mergeCell ref="B44:D44"/>
     <mergeCell ref="B29:F29"/>
@@ -2861,14 +2861,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="33"/>
+    <col min="1" max="16384" width="9.125" style="33"/>
   </cols>
   <sheetData>
     <row r="1" s="34" customFormat="1"/>
@@ -2878,508 +2878,508 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B43" sqref="B43:D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="11.4"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="22.5">
+    <row r="1" spans="1:10" ht="21">
       <c r="A1" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1">
-      <c r="A3" s="69" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
+      <c r="A3" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1">
-      <c r="A4" s="69"/>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
+      <c r="A4" s="67"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="70"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
+      <c r="A5" s="68"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="71"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
+      <c r="A6" s="69"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="71"/>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
+      <c r="A7" s="69"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="71"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
+      <c r="A8" s="69"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="71"/>
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="71"/>
+      <c r="A9" s="69"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="71"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="71"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="71"/>
+      <c r="A10" s="69"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="71"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="71"/>
+      <c r="A11" s="69"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="69"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="71"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
+      <c r="A12" s="69"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="71"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="71"/>
+      <c r="A13" s="69"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="71"/>
-      <c r="B14" s="71"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="71"/>
-      <c r="H14" s="71"/>
-      <c r="I14" s="71"/>
-      <c r="J14" s="71"/>
+      <c r="A14" s="69"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="69"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="71"/>
-      <c r="B15" s="71"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="71"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="71"/>
+      <c r="A15" s="69"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="71"/>
-      <c r="B16" s="71"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
-      <c r="H16" s="71"/>
-      <c r="I16" s="71"/>
-      <c r="J16" s="71"/>
+      <c r="A16" s="69"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="71"/>
-      <c r="B17" s="71"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="71"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="71"/>
+      <c r="A17" s="69"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="69"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="71"/>
-      <c r="B18" s="71"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
+      <c r="A18" s="69"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="71"/>
-      <c r="B19" s="71"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="71"/>
-      <c r="I19" s="71"/>
-      <c r="J19" s="71"/>
+      <c r="A19" s="69"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="71"/>
-      <c r="B20" s="71"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="71"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="71"/>
+      <c r="A20" s="69"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="69"/>
+      <c r="J20" s="69"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="71"/>
-      <c r="B21" s="71"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="71"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="71"/>
+      <c r="A21" s="69"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="69"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="71"/>
-      <c r="B22" s="71"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="71"/>
-      <c r="I22" s="71"/>
-      <c r="J22" s="71"/>
+      <c r="A22" s="69"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="69"/>
+      <c r="J22" s="69"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="71"/>
-      <c r="B23" s="71"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="71"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="71"/>
+      <c r="A23" s="69"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="69"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="69"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="71"/>
-      <c r="B24" s="71"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
+      <c r="A24" s="69"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="71"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="71"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="71"/>
+      <c r="A25" s="69"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="69"/>
+      <c r="I25" s="69"/>
+      <c r="J25" s="69"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="71"/>
-      <c r="B26" s="71"/>
-      <c r="C26" s="71"/>
-      <c r="D26" s="71"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="71"/>
+      <c r="A26" s="69"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="69"/>
+      <c r="I26" s="69"/>
+      <c r="J26" s="69"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="71"/>
-      <c r="B27" s="71"/>
-      <c r="C27" s="71"/>
-      <c r="D27" s="71"/>
-      <c r="E27" s="71"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="71"/>
-      <c r="I27" s="71"/>
-      <c r="J27" s="71"/>
+      <c r="A27" s="69"/>
+      <c r="B27" s="69"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
+      <c r="G27" s="69"/>
+      <c r="H27" s="69"/>
+      <c r="I27" s="69"/>
+      <c r="J27" s="69"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="71"/>
-      <c r="B28" s="71"/>
-      <c r="C28" s="71"/>
-      <c r="D28" s="71"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
+      <c r="A28" s="69"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="69"/>
+      <c r="I28" s="69"/>
+      <c r="J28" s="69"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="71"/>
-      <c r="B29" s="71"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="71"/>
-      <c r="E29" s="71"/>
-      <c r="F29" s="71"/>
-      <c r="G29" s="71"/>
-      <c r="H29" s="71"/>
-      <c r="I29" s="71"/>
-      <c r="J29" s="71"/>
+      <c r="A29" s="69"/>
+      <c r="B29" s="69"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="69"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="69"/>
+      <c r="I29" s="69"/>
+      <c r="J29" s="69"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="71"/>
-      <c r="B30" s="71"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="71"/>
+      <c r="A30" s="69"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="69"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="71"/>
-      <c r="B31" s="71"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="71"/>
-      <c r="E31" s="71"/>
-      <c r="F31" s="71"/>
-      <c r="G31" s="71"/>
-      <c r="H31" s="71"/>
-      <c r="I31" s="71"/>
-      <c r="J31" s="71"/>
+      <c r="A31" s="69"/>
+      <c r="B31" s="69"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="69"/>
+      <c r="I31" s="69"/>
+      <c r="J31" s="69"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="71"/>
-      <c r="B32" s="71"/>
-      <c r="C32" s="71"/>
-      <c r="D32" s="71"/>
-      <c r="E32" s="71"/>
-      <c r="F32" s="71"/>
-      <c r="G32" s="71"/>
-      <c r="H32" s="71"/>
-      <c r="I32" s="71"/>
-      <c r="J32" s="71"/>
+      <c r="A32" s="69"/>
+      <c r="B32" s="69"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="69"/>
+      <c r="G32" s="69"/>
+      <c r="H32" s="69"/>
+      <c r="I32" s="69"/>
+      <c r="J32" s="69"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="71"/>
-      <c r="B33" s="71"/>
-      <c r="C33" s="71"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="71"/>
-      <c r="G33" s="71"/>
-      <c r="H33" s="71"/>
-      <c r="I33" s="71"/>
-      <c r="J33" s="71"/>
+      <c r="A33" s="69"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="69"/>
+      <c r="J33" s="69"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="71"/>
-      <c r="B34" s="71"/>
-      <c r="C34" s="71"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="71"/>
-      <c r="F34" s="71"/>
-      <c r="G34" s="71"/>
-      <c r="H34" s="71"/>
-      <c r="I34" s="71"/>
-      <c r="J34" s="71"/>
+      <c r="A34" s="69"/>
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
+      <c r="J34" s="69"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="71"/>
-      <c r="B35" s="71"/>
-      <c r="C35" s="71"/>
-      <c r="D35" s="71"/>
-      <c r="E35" s="71"/>
-      <c r="F35" s="71"/>
-      <c r="G35" s="71"/>
-      <c r="H35" s="71"/>
-      <c r="I35" s="71"/>
-      <c r="J35" s="71"/>
+      <c r="A35" s="69"/>
+      <c r="B35" s="69"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="69"/>
+      <c r="J35" s="69"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="71"/>
-      <c r="B36" s="71"/>
-      <c r="C36" s="71"/>
-      <c r="D36" s="71"/>
-      <c r="E36" s="71"/>
-      <c r="F36" s="71"/>
-      <c r="G36" s="71"/>
-      <c r="H36" s="71"/>
-      <c r="I36" s="71"/>
-      <c r="J36" s="71"/>
+      <c r="A36" s="69"/>
+      <c r="B36" s="69"/>
+      <c r="C36" s="69"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="69"/>
+      <c r="H36" s="69"/>
+      <c r="I36" s="69"/>
+      <c r="J36" s="69"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="71"/>
-      <c r="B37" s="71"/>
-      <c r="C37" s="71"/>
-      <c r="D37" s="71"/>
-      <c r="E37" s="71"/>
-      <c r="F37" s="71"/>
-      <c r="G37" s="71"/>
-      <c r="H37" s="71"/>
-      <c r="I37" s="71"/>
-      <c r="J37" s="71"/>
+      <c r="A37" s="69"/>
+      <c r="B37" s="69"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="69"/>
+      <c r="H37" s="69"/>
+      <c r="I37" s="69"/>
+      <c r="J37" s="69"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="71"/>
-      <c r="B38" s="71"/>
-      <c r="C38" s="71"/>
-      <c r="D38" s="71"/>
-      <c r="E38" s="71"/>
-      <c r="F38" s="71"/>
-      <c r="G38" s="71"/>
-      <c r="H38" s="71"/>
-      <c r="I38" s="71"/>
-      <c r="J38" s="71"/>
+      <c r="A38" s="69"/>
+      <c r="B38" s="69"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="69"/>
+      <c r="G38" s="69"/>
+      <c r="H38" s="69"/>
+      <c r="I38" s="69"/>
+      <c r="J38" s="69"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="71"/>
-      <c r="B39" s="71"/>
-      <c r="C39" s="71"/>
-      <c r="D39" s="71"/>
-      <c r="E39" s="71"/>
-      <c r="F39" s="71"/>
-      <c r="G39" s="71"/>
-      <c r="H39" s="71"/>
-      <c r="I39" s="71"/>
-      <c r="J39" s="71"/>
+      <c r="A39" s="69"/>
+      <c r="B39" s="69"/>
+      <c r="C39" s="69"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="69"/>
+      <c r="I39" s="69"/>
+      <c r="J39" s="69"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="71"/>
-      <c r="B40" s="71"/>
-      <c r="C40" s="71"/>
-      <c r="D40" s="71"/>
-      <c r="E40" s="71"/>
-      <c r="F40" s="71"/>
-      <c r="G40" s="71"/>
-      <c r="H40" s="71"/>
-      <c r="I40" s="71"/>
-      <c r="J40" s="71"/>
+      <c r="A40" s="69"/>
+      <c r="B40" s="69"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="69"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="69"/>
+      <c r="G40" s="69"/>
+      <c r="H40" s="69"/>
+      <c r="I40" s="69"/>
+      <c r="J40" s="69"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="71"/>
-      <c r="B41" s="71"/>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
-      <c r="E41" s="71"/>
-      <c r="F41" s="71"/>
-      <c r="G41" s="71"/>
-      <c r="H41" s="71"/>
-      <c r="I41" s="71"/>
-      <c r="J41" s="71"/>
+      <c r="A41" s="69"/>
+      <c r="B41" s="69"/>
+      <c r="C41" s="69"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="69"/>
+      <c r="G41" s="69"/>
+      <c r="H41" s="69"/>
+      <c r="I41" s="69"/>
+      <c r="J41" s="69"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="71"/>
-      <c r="B42" s="71"/>
-      <c r="C42" s="71"/>
-      <c r="D42" s="71"/>
-      <c r="E42" s="71"/>
-      <c r="F42" s="71"/>
-      <c r="G42" s="71"/>
-      <c r="H42" s="71"/>
-      <c r="I42" s="71"/>
-      <c r="J42" s="71"/>
+      <c r="A42" s="69"/>
+      <c r="B42" s="69"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="69"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="69"/>
+      <c r="I42" s="69"/>
+      <c r="J42" s="69"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>0</v>
       </c>
       <c r="B43" s="40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" s="40"/>
       <c r="D43" s="40"/>
@@ -3398,18 +3398,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="11.4"/>
   <sheetData>
     <row r="1" spans="1:9" ht="15">
-      <c r="A1" s="72" t="s">
-        <v>73</v>
+      <c r="A1" s="70" t="s">
+        <v>72</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -3420,152 +3420,152 @@
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
     </row>
-    <row r="2" spans="1:9" ht="20.25" thickBot="1">
+    <row r="2" spans="1:9" ht="19.2" thickBot="1">
       <c r="A2" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" t="s">
         <v>75</v>
       </c>
-      <c r="I2" t="s">
+    </row>
+    <row r="3" spans="1:9" ht="15.6" thickBot="1">
+      <c r="A3" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A3" s="5" t="s">
+      <c r="G3" s="26"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.6" thickBot="1">
+      <c r="A4" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="G3" s="26"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A4" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="G4" s="26"/>
     </row>
     <row r="5" spans="1:9" ht="17.25" customHeight="1" thickBot="1">
       <c r="A5" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G5" s="26"/>
       <c r="I5" s="26"/>
     </row>
     <row r="6" spans="1:9" ht="27" customHeight="1" thickBot="1">
-      <c r="A6" s="73" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="74"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
+      <c r="A6" s="71" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
       <c r="G6" s="26"/>
       <c r="I6" s="26"/>
     </row>
-    <row r="8" spans="1:9" ht="20.25" thickBot="1">
+    <row r="8" spans="1:9" ht="19.2" thickBot="1">
       <c r="A8" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.6" thickBot="1">
+      <c r="A9" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A9" s="5" t="s">
+      <c r="G9" s="26"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.6" thickBot="1">
+      <c r="A10" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="G9" s="26"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A10" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
       </c>
       <c r="G10" s="26"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+    <row r="11" spans="1:9" ht="15.6" thickBot="1">
       <c r="A11" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.6" thickBot="1">
+      <c r="A12" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G11" s="26"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A12" s="5" t="s">
+      <c r="G12" s="26"/>
+    </row>
+    <row r="14" spans="1:9" ht="19.2" thickBot="1">
+      <c r="A14" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="G12" s="26"/>
-    </row>
-    <row r="14" spans="1:9" ht="20.25" thickBot="1">
-      <c r="A14" s="29" t="s">
-        <v>86</v>
-      </c>
       <c r="G14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" t="s">
         <v>75</v>
       </c>
-      <c r="I14" t="s">
+    </row>
+    <row r="15" spans="1:9" ht="15.6" thickBot="1">
+      <c r="A15" s="5" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A15" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="G15" s="26"/>
       <c r="I15" s="26"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1">
+    <row r="16" spans="1:9" ht="15.6" thickBot="1">
       <c r="A16" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G16" s="26"/>
       <c r="I16" s="26"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1">
+    <row r="17" spans="1:9" ht="15.6" thickBot="1">
       <c r="A17" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" s="26"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.6" thickBot="1">
+      <c r="A18" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="26"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A18" s="5" t="s">
+      <c r="G18" s="26"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.6" thickBot="1">
+      <c r="A19" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="G18" s="26"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A19" s="5" t="s">
+      <c r="G19" s="26"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.6" thickBot="1">
+      <c r="A20" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="G19" s="26"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A20" s="5" t="s">
-        <v>91</v>
       </c>
       <c r="G20" s="26"/>
       <c r="I20" s="26"/>
     </row>
     <row r="21" spans="1:9" ht="29.25" customHeight="1">
-      <c r="A21" s="75" t="s">
-        <v>92</v>
+      <c r="A21" s="73" t="s">
+        <v>91</v>
       </c>
       <c r="B21" s="38"/>
       <c r="C21" s="38"/>
       <c r="D21" s="38"/>
       <c r="E21" s="38"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1">
+    <row r="22" spans="1:9" ht="15.6" thickBot="1">
       <c r="A22" s="5"/>
     </row>
     <row r="23" spans="1:9" ht="46.5" customHeight="1" thickBot="1">
-      <c r="A23" s="76" t="s">
-        <v>93</v>
-      </c>
-      <c r="B23" s="77"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
+      <c r="A23" s="74" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
       <c r="G23" s="26"/>
     </row>
     <row r="24" spans="1:9" ht="15">
@@ -3573,27 +3573,27 @@
     </row>
     <row r="25" spans="1:9" ht="15">
       <c r="A25" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15">
       <c r="A27" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15">
       <c r="A28" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="B30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E30" s="30"/>
     </row>

</xml_diff>